<commit_message>
Ajusta controle de investimento
</commit_message>
<xml_diff>
--- a/Controle de Investimento.xlsx
+++ b/Controle de Investimento.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inpact2-my.sharepoint.com/personal/lua_impactlegal_com_br/Documents/Área de Trabalho/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://inpact2-my.sharepoint.com/personal/lua_impactlegal_com_br/Documents/Documentos/GitHub/Lua/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="570" documentId="11_AD4D361C20488DEA4E38A077DC5B40AA5BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{682B3F2C-FB14-4A88-8D40-E87521F0D096}"/>
+  <xr:revisionPtr revIDLastSave="574" documentId="11_AD4D361C20488DEA4E38A077DC5B40AA5BDEDD80" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E02BD0FF-FE36-4E6F-95A6-AE278F1447D1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP" sheetId="2" r:id="rId1"/>
@@ -155,7 +155,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
-    <numFmt numFmtId="168" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -815,11 +815,11 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="8" fontId="7" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -839,25 +839,7 @@
     <xf numFmtId="8" fontId="7" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -871,142 +853,157 @@
     </xf>
     <xf numFmtId="8" fontId="7" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="168" fontId="7" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="8" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="4" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="4" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutro" xfId="2" builtinId="28"/>
@@ -1350,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7E8E25-E1FF-473F-99AC-95E82656C14C}">
   <dimension ref="A10:F54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,103 +1365,103 @@
   <sheetData>
     <row r="10" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="12"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="62"/>
     </row>
     <row r="12" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="17">
+      <c r="C12" s="55"/>
+      <c r="D12" s="11">
         <v>10100</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="37"/>
-      <c r="D13" s="19">
+      <c r="C13" s="57"/>
+      <c r="D13" s="13">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="39">
+      <c r="C14" s="59"/>
+      <c r="D14" s="19">
         <f>Salario*30%</f>
         <v>3030</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:4" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="14"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="65"/>
     </row>
     <row r="17" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="17">
-        <v>2440</v>
+      <c r="C17" s="67"/>
+      <c r="D17" s="11">
+        <v>3030</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="18">
+      <c r="C18" s="69"/>
+      <c r="D18" s="12">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="19">
+      <c r="C19" s="69"/>
+      <c r="D19" s="13">
         <v>1.0789999999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="20">
+      <c r="C20" s="71"/>
+      <c r="D20" s="14">
         <f>FV(Taxa_mensal,Quantidade_anos*12,Valor_investir_mês*-1)</f>
-        <v>204415.67015630985</v>
+        <v>253844.04941541757</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="21">
+      <c r="C21" s="73"/>
+      <c r="D21" s="15">
         <f>D20*Rendimento_carteira</f>
-        <v>1226.4940209378592</v>
+        <v>1523.0642964925055</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="16"/>
+      <c r="C23" s="64"/>
       <c r="D23" s="3" t="s">
         <v>12</v>
       </c>
@@ -1473,198 +1470,198 @@
       <c r="A24" s="2">
         <v>2</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C24" s="5">
         <f>FV($D$19,$A24*12,$D$17*-1)</f>
-        <v>66435.410606254329</v>
+        <v>82499.710711865002</v>
       </c>
       <c r="D24" s="6">
         <f>C24*Rendimento_carteira</f>
-        <v>398.61246363752599</v>
+        <v>494.99826427119001</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>5</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C25" s="7">
         <f>FV($D$19,$A25*12,$D$17*-1)</f>
-        <v>204415.67015630985</v>
+        <v>253844.04941541757</v>
       </c>
       <c r="D25" s="8">
         <f>C25*Rendimento_carteira</f>
-        <v>1226.4940209378592</v>
+        <v>1523.0642964925055</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>10</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="7">
         <f>FV($D$19,$A26*12,$D$17*-1)</f>
-        <v>593613.4785736202</v>
+        <v>737151.16396642174</v>
       </c>
       <c r="D26" s="8">
         <f>C26*Rendimento_carteira</f>
-        <v>3561.6808714417211</v>
+        <v>4422.9069837985307</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>20</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C27" s="7">
         <f>FV($D$19,$A27*12,$D$17*-1)</f>
-        <v>2745484.0962368767</v>
+        <v>3409351.1522941543</v>
       </c>
       <c r="D27" s="8">
         <f>C27*Rendimento_carteira</f>
-        <v>16472.904577421261</v>
+        <v>20456.106913764925</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>30</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C28" s="9">
         <f>FV($D$19,$A28*12,$D$17*-1)</f>
-        <v>10546093.958211504</v>
+        <v>13096174.054664286</v>
       </c>
       <c r="D28" s="10">
         <f>C28*Rendimento_carteira</f>
-        <v>63276.563749269022</v>
+        <v>78577.044327985714</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="41" t="s">
+      <c r="C30" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="42"/>
+      <c r="D30" s="51"/>
     </row>
     <row r="31" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="44">
+      <c r="C31" s="52">
         <f>Valor_investir_mês</f>
-        <v>2440</v>
-      </c>
-      <c r="D31" s="45"/>
+        <v>3030</v>
+      </c>
+      <c r="D31" s="53"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="49" t="s">
+      <c r="B33" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="50" t="s">
+      <c r="C33" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D33" s="51" t="s">
+      <c r="D33" s="27" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="47" t="s">
+      <c r="B34" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="48">
+      <c r="C34" s="24">
         <f>VLOOKUP($C$30&amp;"-"&amp;B34,'Tabela acessória'!A2:D20,4,FALSE)</f>
         <v>0.5</v>
       </c>
-      <c r="D34" s="56">
+      <c r="D34" s="32">
         <f>$C$31*C34</f>
-        <v>1220</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="48">
+      <c r="C35" s="24">
         <f>VLOOKUP($C$30&amp;"-"&amp;B35,'Tabela acessória'!A3:D21,4,FALSE)</f>
         <v>0.1</v>
       </c>
-      <c r="D35" s="57">
+      <c r="D35" s="33">
         <f t="shared" ref="D35:D39" si="0">$C$31*C35</f>
-        <v>244</v>
+        <v>303</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="48">
+      <c r="C36" s="24">
         <f>VLOOKUP($C$30&amp;"-"&amp;B36,'Tabela acessória'!A4:D22,4,FALSE)</f>
         <v>0.05</v>
       </c>
-      <c r="D36" s="57">
+      <c r="D36" s="33">
         <f t="shared" si="0"/>
-        <v>122</v>
+        <v>151.5</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="46" t="s">
+      <c r="B37" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="48">
+      <c r="C37" s="24">
         <f>VLOOKUP($C$30&amp;"-"&amp;B37,'Tabela acessória'!A5:D23,4,FALSE)</f>
         <v>0.05</v>
       </c>
-      <c r="D37" s="57">
+      <c r="D37" s="33">
         <f t="shared" si="0"/>
-        <v>122</v>
+        <v>151.5</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="48">
+      <c r="C38" s="24">
         <f>VLOOKUP($C$30&amp;"-"&amp;B38,'Tabela acessória'!A6:D24,4,FALSE)</f>
         <v>0.2</v>
       </c>
-      <c r="D38" s="57">
+      <c r="D38" s="33">
         <f t="shared" si="0"/>
-        <v>488</v>
+        <v>606</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="52" t="s">
+      <c r="B39" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="48">
+      <c r="C39" s="24">
         <f>VLOOKUP($C$30&amp;"-"&amp;B39,'Tabela acessória'!A7:D25,4,FALSE)</f>
         <v>0.1</v>
       </c>
-      <c r="D39" s="58">
+      <c r="D39" s="34">
         <f t="shared" si="0"/>
-        <v>244</v>
+        <v>303</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="53"/>
-      <c r="C40" s="54"/>
-      <c r="D40" s="55">
+      <c r="B40" s="29"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="31">
         <f>SUM(D34:D39)</f>
-        <v>2440</v>
+        <v>3030</v>
       </c>
     </row>
     <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1675,11 +1672,6 @@
     <row r="54" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B23:C23"/>
@@ -1688,6 +1680,11 @@
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C30" xr:uid="{A589337B-A333-45DA-B6EE-7CAFAE2B695D}">
@@ -1716,286 +1713,286 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="49" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="str">
+      <c r="A3" s="35" t="str">
         <f>$B3&amp;"-"&amp;C3</f>
         <v>Conservador-PAPEL</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="61">
+      <c r="D3" s="37">
         <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="59" t="str">
+      <c r="A4" s="35" t="str">
         <f t="shared" ref="A4:A20" si="0">$B4&amp;"-"&amp;C4</f>
         <v>Conservador-TIJOLO</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="61">
+      <c r="D4" s="37">
         <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="str">
+      <c r="A5" s="35" t="str">
         <f t="shared" si="0"/>
         <v>Conservador-HÍBRIDOS</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="61">
+      <c r="D5" s="37">
         <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="str">
+      <c r="A6" s="35" t="str">
         <f t="shared" si="0"/>
         <v>Conservador-FOFs</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="61">
+      <c r="D6" s="37">
         <v>0.1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="59" t="str">
+      <c r="A7" s="35" t="str">
         <f t="shared" si="0"/>
         <v>Conservador-DESENVOLVIMENTO</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="61">
+      <c r="D7" s="37">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="68" t="str">
+      <c r="A8" s="43" t="str">
         <f t="shared" si="0"/>
         <v>Conservador-HOTELARIAS</v>
       </c>
-      <c r="B8" s="69" t="s">
+      <c r="B8" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="70" t="s">
+      <c r="C8" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="71">
+      <c r="D8" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="64" t="str">
+      <c r="A9" s="39" t="str">
         <f t="shared" si="0"/>
         <v>Moderado-PAPEL</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="66" t="s">
+      <c r="C9" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="67">
+      <c r="D9" s="42">
         <v>0.32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="59" t="str">
+      <c r="A10" s="35" t="str">
         <f t="shared" si="0"/>
         <v>Moderado-TIJOLO</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="62">
+      <c r="D10" s="37">
         <v>0.35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="59" t="str">
+      <c r="A11" s="35" t="str">
         <f t="shared" si="0"/>
         <v>Moderado-HÍBRIDOS</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="60" t="s">
+      <c r="C11" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="62">
+      <c r="D11" s="37">
         <v>0.08</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="59" t="str">
+      <c r="A12" s="35" t="str">
         <f t="shared" si="0"/>
         <v>Moderado-FOFs</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="60" t="s">
+      <c r="C12" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="62">
+      <c r="D12" s="37">
         <v>0.05</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="59" t="str">
+      <c r="A13" s="35" t="str">
         <f t="shared" si="0"/>
         <v>Moderado-DESENVOLVIMENTO</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="60" t="s">
+      <c r="C13" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="61">
+      <c r="D13" s="37">
         <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="68" t="str">
+      <c r="A14" s="43" t="str">
         <f t="shared" si="0"/>
         <v>Moderado-HOTELARIAS</v>
       </c>
-      <c r="B14" s="69" t="s">
+      <c r="B14" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="70" t="s">
+      <c r="C14" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="73">
+      <c r="D14" s="48">
         <v>0.1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="64" t="str">
+      <c r="A15" s="39" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo-PAPEL</v>
       </c>
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="66" t="s">
+      <c r="C15" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="72">
+      <c r="D15" s="47">
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="59" t="str">
+      <c r="A16" s="35" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo-TIJOLO</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="63">
+      <c r="D16" s="38">
         <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="59" t="str">
+      <c r="A17" s="35" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo-HÍBRIDOS</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="63">
+      <c r="D17" s="38">
         <v>0.05</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="59" t="str">
+      <c r="A18" s="35" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo-FOFs</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="63">
+      <c r="D18" s="38">
         <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="59" t="str">
+      <c r="A19" s="35" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo-DESENVOLVIMENTO</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="60" t="s">
+      <c r="C19" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="63">
+      <c r="D19" s="38">
         <v>0.2</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="59" t="str">
+      <c r="A20" s="35" t="str">
         <f t="shared" si="0"/>
         <v>Agressivo-HOTELARIAS</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="63">
+      <c r="D20" s="38">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>